<commit_message>
Add past version history
</commit_message>
<xml_diff>
--- a/documents/document_list/文書管理台帳.xlsx
+++ b/documents/document_list/文書管理台帳.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_7BDD26FB8B166F1FFE6CB395D37497EFC86A3294" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFA1241E-940C-4526-9E3D-8ED926173241}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="11_7BDD26FB8B166F1FFE6CB395D37497EFC86A3294" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{219010F6-9ED0-41B2-B25B-954E1CF5ECA1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>文書番号</t>
   </si>
@@ -179,6 +179,13 @@
       <t>ケイカクショ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第2.0版</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/azreus906/10031s0000/tree/main/documents/plan</t>
   </si>
 </sst>
 </file>
@@ -871,10 +878,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -943,7 +950,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -954,61 +961,69 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>5</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="G4" s="16">
+        <v>45467</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="20.100000000000001" customHeight="1">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="16">
+        <v>45467</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="20.100000000000001" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" s="12" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>8</v>
@@ -1017,16 +1032,16 @@
         <v>12</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="7"/>
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>8</v>
@@ -1039,15 +1054,41 @@
       <c r="G8" s="7"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1">
-      <c r="C9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" s="14" customFormat="1">
-      <c r="C10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="G10" s="15"/>
+    <row r="9" spans="1:8" s="13" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" s="13" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" s="14" customFormat="1">
       <c r="C11" s="15"/>
@@ -1164,19 +1205,30 @@
       <c r="E33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="3:7">
-      <c r="F34" s="14"/>
+    <row r="34" spans="3:7" s="14" customFormat="1">
+      <c r="C34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="3:7" s="14" customFormat="1">
+      <c r="C35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="G35" s="15"/>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="F36" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{B870529B-B918-4349-A6D0-AD6A97E5C8A6}"/>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{B870529B-B918-4349-A6D0-AD6A97E5C8A6}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{EB1D383A-17C3-4F2B-82FD-F08176674C0F}"/>
+    <hyperlink ref="F4:F5" r:id="rId3" display="https://github.com/azreus906/10031s0001/tree/main/documents/plan" xr:uid="{543D6357-6F63-463E-8259-A11834A2FD3E}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="1.1811023622047245" bottom="1.1811023622047245" header="0.86614173228346458" footer="0.86614173228346458"/>
-  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="240" verticalDpi="240" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="240" verticalDpi="240" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>